<commit_message>
#47 Major revamp of SignTrainerUIFragment class. Video sizes are now computed instead of defined in the layout xml file.
</commit_message>
<xml_diff>
--- a/hardware-profiles/DPI-Pixel-Converter.xlsx
+++ b/hardware-profiles/DPI-Pixel-Converter.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>dip</t>
   </si>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G11"/>
+  <dimension ref="A3:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,19 +471,19 @@
         <v>120</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D24" si="0">$C5/160</f>
+        <f t="shared" ref="D5:D11" si="0">$C5/160</f>
         <v>0.75</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E24" si="1">$B5*$D5</f>
+        <f t="shared" ref="E5:E11" si="1">$B5*$D5</f>
         <v>240</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F24" si="2">$E5/$C5</f>
+        <f t="shared" ref="F5:F11" si="2">$E5/$C5</f>
         <v>2</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" ref="G5:G24" si="3">IF(ISEVEN(ROW()),SQRT(($F5*$F5)+($F6*$F6)),"")</f>
+        <f t="shared" ref="G5:G11" si="3">IF(ISEVEN(ROW()),SQRT(($F5*$F5)+($F6*$F6)),"")</f>
         <v/>
       </c>
     </row>
@@ -647,6 +647,49 @@
       <c r="G11" t="str">
         <f t="shared" si="3"/>
         <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>426</v>
+      </c>
+      <c r="C13">
+        <v>160</v>
+      </c>
+      <c r="D13">
+        <v>0.75</v>
+      </c>
+      <c r="E13">
+        <v>319.5</v>
+      </c>
+      <c r="F13">
+        <v>2.6625000000000001</v>
+      </c>
+      <c r="G13">
+        <v>3.330000938</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>320</v>
+      </c>
+      <c r="C14">
+        <v>160</v>
+      </c>
+      <c r="D14">
+        <v>0.75</v>
+      </c>
+      <c r="E14">
+        <v>240</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>